<commit_message>
Deprecate Type 1 diabetes mellitus, Type 2 diabetes mellitus, Diabetic ketoacidosis in favor of Gestational diabetes mellitus, diabetes mellitus
201254000,201820000,201254000,Type 1 diabetes mellitus
201826000,201820000,201826000,Type 2 diabetes mellitus
443727000,201820000,443727000,Diabetic ketoacidosis
4024659000,201820000,4024659000,Gestational diabetes mellitus
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\github\ohdsi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\github\ohdsi\PhenotypeLibrary\extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6057,7 +6057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C799" sqref="C799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11885,7 +11885,7 @@
     </row>
     <row r="206" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>201254000</v>
+        <v>201820000</v>
       </c>
       <c r="B206">
         <v>17693</v>
@@ -11914,7 +11914,7 @@
     </row>
     <row r="207" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>201254000</v>
+        <v>201820000</v>
       </c>
       <c r="B207">
         <v>17692</v>
@@ -11943,7 +11943,7 @@
     </row>
     <row r="208" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>201254000</v>
+        <v>201820000</v>
       </c>
       <c r="B208">
         <v>18999</v>
@@ -12378,7 +12378,7 @@
     </row>
     <row r="223" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B223">
         <v>17695</v>
@@ -12407,7 +12407,7 @@
     </row>
     <row r="224" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B224">
         <v>17694</v>
@@ -12436,7 +12436,7 @@
     </row>
     <row r="225" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B225">
         <v>17720</v>
@@ -12459,7 +12459,7 @@
     </row>
     <row r="226" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B226">
         <v>18933</v>
@@ -12485,7 +12485,7 @@
     </row>
     <row r="227" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B227">
         <v>18934</v>
@@ -12511,7 +12511,7 @@
     </row>
     <row r="228" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B228">
         <v>18972</v>
@@ -12540,7 +12540,7 @@
     </row>
     <row r="229" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B229">
         <v>18964</v>
@@ -12569,7 +12569,7 @@
     </row>
     <row r="230" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>201826000</v>
+        <v>201820000</v>
       </c>
       <c r="B230">
         <v>19031</v>
@@ -22295,7 +22295,7 @@
     </row>
     <row r="578" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A578">
-        <v>443727000</v>
+        <v>201820000</v>
       </c>
       <c r="B578">
         <v>17467</v>
@@ -22324,7 +22324,7 @@
     </row>
     <row r="579" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A579">
-        <v>443727000</v>
+        <v>201820000</v>
       </c>
       <c r="B579">
         <v>17466</v>
@@ -22927,7 +22927,7 @@
     </row>
     <row r="600" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A600">
-        <v>4024659000</v>
+        <v>201820000</v>
       </c>
       <c r="B600">
         <v>17798</v>
@@ -22956,7 +22956,7 @@
     </row>
     <row r="601" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A601">
-        <v>4024659000</v>
+        <v>201820000</v>
       </c>
       <c r="B601">
         <v>17797</v>
@@ -22985,7 +22985,7 @@
     </row>
     <row r="602" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A602">
-        <v>4024659000</v>
+        <v>201820000</v>
       </c>
       <c r="B602">
         <v>17762</v>

</xml_diff>

<commit_message>
Deprecate clinical signs and symptoms phenotype and group into 4094294000,Clinical Signs and Symptoms
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -6057,7 +6057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C799" sqref="C799"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6107,7 +6107,7 @@
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>24134000</v>
+        <v>4094294000</v>
       </c>
       <c r="B2">
         <v>17595</v>
@@ -6136,7 +6136,7 @@
     </row>
     <row r="3" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>24134000</v>
+        <v>4094294000</v>
       </c>
       <c r="B3">
         <v>17594</v>
@@ -6165,7 +6165,7 @@
     </row>
     <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>24134000</v>
+        <v>4094294000</v>
       </c>
       <c r="B4">
         <v>18994</v>
@@ -6423,7 +6423,7 @@
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>31317000</v>
+        <v>4094294000</v>
       </c>
       <c r="B13">
         <v>17471</v>
@@ -6452,7 +6452,7 @@
     </row>
     <row r="14" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>31317000</v>
+        <v>4094294000</v>
       </c>
       <c r="B14">
         <v>17470</v>
@@ -6481,7 +6481,7 @@
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>31317000</v>
+        <v>4094294000</v>
       </c>
       <c r="B15">
         <v>17871</v>
@@ -6510,7 +6510,7 @@
     </row>
     <row r="16" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>31967000</v>
+        <v>4094294000</v>
       </c>
       <c r="B16">
         <v>17593</v>
@@ -6539,7 +6539,7 @@
     </row>
     <row r="17" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>31967000</v>
+        <v>4094294000</v>
       </c>
       <c r="B17">
         <v>17592</v>
@@ -6568,7 +6568,7 @@
     </row>
     <row r="18" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>31967000</v>
+        <v>4094294000</v>
       </c>
       <c r="B18">
         <v>18996</v>
@@ -6594,7 +6594,7 @@
     </row>
     <row r="19" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>75860000</v>
+        <v>4094294000</v>
       </c>
       <c r="B19">
         <v>17451</v>
@@ -6623,7 +6623,7 @@
     </row>
     <row r="20" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>75860000</v>
+        <v>4094294000</v>
       </c>
       <c r="B20">
         <v>17450</v>
@@ -6652,7 +6652,7 @@
     </row>
     <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>75860000</v>
+        <v>4094294000</v>
       </c>
       <c r="B21">
         <v>18997</v>
@@ -6736,7 +6736,7 @@
     </row>
     <row r="24" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>77074000</v>
+        <v>4094294000</v>
       </c>
       <c r="B24">
         <v>17537</v>
@@ -6765,7 +6765,7 @@
     </row>
     <row r="25" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>77074000</v>
+        <v>4094294000</v>
       </c>
       <c r="B25">
         <v>17536</v>
@@ -8927,7 +8927,7 @@
     </row>
     <row r="101" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>137977000</v>
+        <v>4094294000</v>
       </c>
       <c r="B101">
         <v>17535</v>
@@ -8956,7 +8956,7 @@
     </row>
     <row r="102" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>137977000</v>
+        <v>4094294000</v>
       </c>
       <c r="B102">
         <v>17534</v>
@@ -10547,7 +10547,7 @@
     </row>
     <row r="158" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>194133000</v>
+        <v>4094294000</v>
       </c>
       <c r="B158">
         <v>17551</v>
@@ -10576,7 +10576,7 @@
     </row>
     <row r="159" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>194133000</v>
+        <v>4094294000</v>
       </c>
       <c r="B159">
         <v>17550</v>
@@ -10747,7 +10747,7 @@
     </row>
     <row r="165" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>196523000</v>
+        <v>4094294000</v>
       </c>
       <c r="B165">
         <v>17469</v>
@@ -10776,7 +10776,7 @@
     </row>
     <row r="166" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>196523000</v>
+        <v>4094294000</v>
       </c>
       <c r="B166">
         <v>17468</v>
@@ -10805,7 +10805,7 @@
     </row>
     <row r="167" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>196523000</v>
+        <v>4094294000</v>
       </c>
       <c r="B167">
         <v>17841</v>
@@ -10834,7 +10834,7 @@
     </row>
     <row r="168" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>196523000</v>
+        <v>4094294000</v>
       </c>
       <c r="B168">
         <v>17844</v>
@@ -10863,7 +10863,7 @@
     </row>
     <row r="169" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>196523000</v>
+        <v>4094294000</v>
       </c>
       <c r="B169">
         <v>19002</v>
@@ -11633,7 +11633,7 @@
     </row>
     <row r="197" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>200219000</v>
+        <v>4094294000</v>
       </c>
       <c r="B197">
         <v>17375</v>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="198" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>200219000</v>
+        <v>4094294000</v>
       </c>
       <c r="B198">
         <v>17374</v>
@@ -12705,7 +12705,7 @@
     </row>
     <row r="235" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>254761000</v>
+        <v>4094294000</v>
       </c>
       <c r="B235">
         <v>17453</v>
@@ -12734,7 +12734,7 @@
     </row>
     <row r="236" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>254761000</v>
+        <v>4094294000</v>
       </c>
       <c r="B236">
         <v>17452</v>
@@ -12763,7 +12763,7 @@
     </row>
     <row r="237" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>254761000</v>
+        <v>4094294000</v>
       </c>
       <c r="B237">
         <v>17722</v>
@@ -13553,7 +13553,7 @@
     </row>
     <row r="266" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266">
-        <v>312437000</v>
+        <v>4094294000</v>
       </c>
       <c r="B266">
         <v>17473</v>
@@ -13582,7 +13582,7 @@
     </row>
     <row r="267" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267">
-        <v>312437000</v>
+        <v>4094294000</v>
       </c>
       <c r="B267">
         <v>17472</v>
@@ -13611,7 +13611,7 @@
     </row>
     <row r="268" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268">
-        <v>312437000</v>
+        <v>4094294000</v>
       </c>
       <c r="B268">
         <v>17725</v>
@@ -15803,7 +15803,7 @@
     </row>
     <row r="347" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A347">
-        <v>374377000</v>
+        <v>4094294000</v>
       </c>
       <c r="B347">
         <v>18687</v>
@@ -15832,7 +15832,7 @@
     </row>
     <row r="348" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A348">
-        <v>374377000</v>
+        <v>4094294000</v>
       </c>
       <c r="B348">
         <v>18686</v>
@@ -16359,7 +16359,7 @@
     </row>
     <row r="367" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A367">
-        <v>378253000</v>
+        <v>4094294000</v>
       </c>
       <c r="B367">
         <v>17501</v>
@@ -16388,7 +16388,7 @@
     </row>
     <row r="368" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A368">
-        <v>378253000</v>
+        <v>4094294000</v>
       </c>
       <c r="B368">
         <v>17500</v>
@@ -16417,7 +16417,7 @@
     </row>
     <row r="369" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A369">
-        <v>378253000</v>
+        <v>4094294000</v>
       </c>
       <c r="B369">
         <v>19003</v>
@@ -17721,7 +17721,7 @@
     </row>
     <row r="415" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415">
-        <v>433595000</v>
+        <v>4094294000</v>
       </c>
       <c r="B415">
         <v>17475</v>
@@ -17750,7 +17750,7 @@
     </row>
     <row r="416" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416">
-        <v>433595000</v>
+        <v>4094294000</v>
       </c>
       <c r="B416">
         <v>17474</v>
@@ -18564,7 +18564,7 @@
     </row>
     <row r="445" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445">
-        <v>436096000</v>
+        <v>4094294000</v>
       </c>
       <c r="B445">
         <v>17447</v>
@@ -18593,7 +18593,7 @@
     </row>
     <row r="446" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446">
-        <v>436096000</v>
+        <v>4094294000</v>
       </c>
       <c r="B446">
         <v>17446</v>
@@ -19077,7 +19077,7 @@
     </row>
     <row r="463" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A463">
-        <v>436962000</v>
+        <v>4094294000</v>
       </c>
       <c r="B463">
         <v>17533</v>
@@ -19106,7 +19106,7 @@
     </row>
     <row r="464" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A464">
-        <v>436962000</v>
+        <v>4094294000</v>
       </c>
       <c r="B464">
         <v>17532</v>
@@ -19135,7 +19135,7 @@
     </row>
     <row r="465" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A465">
-        <v>436962000</v>
+        <v>4094294000</v>
       </c>
       <c r="B465">
         <v>17869</v>
@@ -19161,7 +19161,7 @@
     </row>
     <row r="466" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A466">
-        <v>436962000</v>
+        <v>4094294000</v>
       </c>
       <c r="B466">
         <v>17870</v>
@@ -19911,7 +19911,7 @@
     </row>
     <row r="493" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A493">
-        <v>437312000</v>
+        <v>4094294000</v>
       </c>
       <c r="B493">
         <v>18740</v>
@@ -19940,7 +19940,7 @@
     </row>
     <row r="494" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A494">
-        <v>437312000</v>
+        <v>4094294000</v>
       </c>
       <c r="B494">
         <v>18739</v>
@@ -19969,7 +19969,7 @@
     </row>
     <row r="495" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A495">
-        <v>437312000</v>
+        <v>4094294000</v>
       </c>
       <c r="B495">
         <v>18770</v>
@@ -20050,7 +20050,7 @@
     </row>
     <row r="498" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A498">
-        <v>437663000</v>
+        <v>4094294000</v>
       </c>
       <c r="B498">
         <v>17483</v>
@@ -20079,7 +20079,7 @@
     </row>
     <row r="499" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A499">
-        <v>437663000</v>
+        <v>4094294000</v>
       </c>
       <c r="B499">
         <v>17482</v>
@@ -20108,7 +20108,7 @@
     </row>
     <row r="500" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A500">
-        <v>437663000</v>
+        <v>4094294000</v>
       </c>
       <c r="B500">
         <v>17721</v>
@@ -20679,7 +20679,7 @@
     </row>
     <row r="520" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A520">
-        <v>440377000</v>
+        <v>4094294000</v>
       </c>
       <c r="B520">
         <v>18685</v>
@@ -20708,7 +20708,7 @@
     </row>
     <row r="521" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A521">
-        <v>440377000</v>
+        <v>4094294000</v>
       </c>
       <c r="B521">
         <v>18684</v>
@@ -21496,7 +21496,7 @@
     </row>
     <row r="549" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A549">
-        <v>441408000</v>
+        <v>4094294000</v>
       </c>
       <c r="B549">
         <v>17713</v>
@@ -21525,7 +21525,7 @@
     </row>
     <row r="550" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A550">
-        <v>441408000</v>
+        <v>4094294000</v>
       </c>
       <c r="B550">
         <v>17712</v>
@@ -21554,7 +21554,7 @@
     </row>
     <row r="551" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A551">
-        <v>441408000</v>
+        <v>4094294000</v>
       </c>
       <c r="B551">
         <v>19005</v>
@@ -21580,7 +21580,7 @@
     </row>
     <row r="552" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A552">
-        <v>441542000</v>
+        <v>4094294000</v>
       </c>
       <c r="B552">
         <v>17407</v>
@@ -21609,7 +21609,7 @@
     </row>
     <row r="553" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A553">
-        <v>441542000</v>
+        <v>4094294000</v>
       </c>
       <c r="B553">
         <v>17406</v>
@@ -21638,7 +21638,7 @@
     </row>
     <row r="554" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A554">
-        <v>441542000</v>
+        <v>4094294000</v>
       </c>
       <c r="B554">
         <v>17826</v>
@@ -21664,7 +21664,7 @@
     </row>
     <row r="555" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A555">
-        <v>441542000</v>
+        <v>4094294000</v>
       </c>
       <c r="B555">
         <v>17842</v>
@@ -21806,7 +21806,7 @@
     </row>
     <row r="560" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A560">
-        <v>442752000</v>
+        <v>4094294000</v>
       </c>
       <c r="B560">
         <v>17808</v>
@@ -21835,7 +21835,7 @@
     </row>
     <row r="561" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A561">
-        <v>442752000</v>
+        <v>4094294000</v>
       </c>
       <c r="B561">
         <v>17807</v>
@@ -21864,7 +21864,7 @@
     </row>
     <row r="562" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A562">
-        <v>442752000</v>
+        <v>4094294000</v>
       </c>
       <c r="B562">
         <v>17723</v>
@@ -22411,7 +22411,7 @@
     </row>
     <row r="582" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A582">
-        <v>444070000</v>
+        <v>4094294000</v>
       </c>
       <c r="B582">
         <v>17683</v>
@@ -22440,7 +22440,7 @@
     </row>
     <row r="583" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A583">
-        <v>444070000</v>
+        <v>4094294000</v>
       </c>
       <c r="B583">
         <v>17682</v>
@@ -25256,7 +25256,7 @@
     </row>
     <row r="683" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A683">
-        <v>4169095000</v>
+        <v>4094294000</v>
       </c>
       <c r="B683">
         <v>17431</v>
@@ -25285,7 +25285,7 @@
     </row>
     <row r="684" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A684">
-        <v>4169095000</v>
+        <v>4094294000</v>
       </c>
       <c r="B684">
         <v>17430</v>
@@ -25314,7 +25314,7 @@
     </row>
     <row r="685" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A685">
-        <v>4169095000</v>
+        <v>4094294000</v>
       </c>
       <c r="B685">
         <v>17735</v>
@@ -25337,7 +25337,7 @@
     </row>
     <row r="686" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A686">
-        <v>4169095000</v>
+        <v>4094294000</v>
       </c>
       <c r="B686">
         <v>7404</v>
@@ -25708,7 +25708,7 @@
     </row>
     <row r="699" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A699">
-        <v>4185711000</v>
+        <v>4094294000</v>
       </c>
       <c r="B699">
         <v>17802</v>
@@ -25737,7 +25737,7 @@
     </row>
     <row r="700" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A700">
-        <v>4185711000</v>
+        <v>4094294000</v>
       </c>
       <c r="B700">
         <v>17801</v>
@@ -25908,7 +25908,7 @@
     </row>
     <row r="706" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A706">
-        <v>4223659000</v>
+        <v>4094294000</v>
       </c>
       <c r="B706">
         <v>18645</v>
@@ -25937,7 +25937,7 @@
     </row>
     <row r="707" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A707">
-        <v>4223659000</v>
+        <v>4094294000</v>
       </c>
       <c r="B707">
         <v>18644</v>
@@ -25966,7 +25966,7 @@
     </row>
     <row r="708" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A708">
-        <v>4223659000</v>
+        <v>4094294000</v>
       </c>
       <c r="B708">
         <v>17724</v>
@@ -26568,7 +26568,7 @@
     </row>
     <row r="730" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A730">
-        <v>4272240000</v>
+        <v>4094294000</v>
       </c>
       <c r="B730">
         <v>17553</v>
@@ -26597,7 +26597,7 @@
     </row>
     <row r="731" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A731">
-        <v>4272240000</v>
+        <v>4094294000</v>
       </c>
       <c r="B731">
         <v>17552</v>
@@ -28109,7 +28109,7 @@
     </row>
     <row r="785" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A785">
-        <v>43530714000</v>
+        <v>4094294000</v>
       </c>
       <c r="B785">
         <v>17810</v>
@@ -28138,7 +28138,7 @@
     </row>
     <row r="786" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A786">
-        <v>43530714000</v>
+        <v>4094294000</v>
       </c>
       <c r="B786">
         <v>17809</v>
@@ -28167,7 +28167,7 @@
     </row>
     <row r="787" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A787">
-        <v>43530714000</v>
+        <v>4094294000</v>
       </c>
       <c r="B787">
         <v>17726</v>
@@ -28190,7 +28190,7 @@
     </row>
     <row r="788" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A788">
-        <v>44784217000</v>
+        <v>4094294000</v>
       </c>
       <c r="B788">
         <v>18627</v>

</xml_diff>

<commit_message>
Group allergy, asthma, atopic dermatitis, angioedema into hypersensitivty
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -6057,7 +6057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="E544" sqref="E544"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8391,7 +8391,7 @@
     </row>
     <row r="82" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B82">
         <v>17413</v>
@@ -8420,7 +8420,7 @@
     </row>
     <row r="83" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B83">
         <v>17412</v>
@@ -8449,7 +8449,7 @@
     </row>
     <row r="84" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B84">
         <v>12800</v>
@@ -8475,7 +8475,7 @@
     </row>
     <row r="85" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B85">
         <v>17143</v>
@@ -8501,7 +8501,7 @@
     </row>
     <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B86">
         <v>18858</v>
@@ -8530,7 +8530,7 @@
     </row>
     <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B87">
         <v>18859</v>
@@ -8559,7 +8559,7 @@
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B88">
         <v>18860</v>
@@ -8588,7 +8588,7 @@
     </row>
     <row r="89" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B89">
         <v>18861</v>
@@ -8617,7 +8617,7 @@
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B90">
         <v>18862</v>
@@ -8646,7 +8646,7 @@
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B91">
         <v>18863</v>
@@ -8675,7 +8675,7 @@
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B92">
         <v>18864</v>
@@ -8704,7 +8704,7 @@
     </row>
     <row r="93" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>133834000</v>
+        <v>43021226000</v>
       </c>
       <c r="B93">
         <v>18865</v>
@@ -12994,7 +12994,7 @@
     </row>
     <row r="246" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246">
-        <v>257007000</v>
+        <v>43021226000</v>
       </c>
       <c r="B246">
         <v>17391</v>
@@ -13023,7 +13023,7 @@
     </row>
     <row r="247" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>257007000</v>
+        <v>43021226000</v>
       </c>
       <c r="B247">
         <v>17390</v>
@@ -17356,7 +17356,7 @@
     </row>
     <row r="402" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402">
-        <v>432791000</v>
+        <v>43021226000</v>
       </c>
       <c r="B402">
         <v>17786</v>
@@ -17385,7 +17385,7 @@
     </row>
     <row r="403" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403">
-        <v>432791000</v>
+        <v>43021226000</v>
       </c>
       <c r="B403">
         <v>17785</v>
@@ -17414,7 +17414,7 @@
     </row>
     <row r="404" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404">
-        <v>432791000</v>
+        <v>43021226000</v>
       </c>
       <c r="B404">
         <v>7377</v>
@@ -21325,7 +21325,7 @@
     </row>
     <row r="543" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A543">
-        <v>441202000</v>
+        <v>43021226000</v>
       </c>
       <c r="B543">
         <v>18620</v>
@@ -21354,7 +21354,7 @@
     </row>
     <row r="544" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A544">
-        <v>441202000</v>
+        <v>43021226000</v>
       </c>
       <c r="B544">
         <v>18619</v>
@@ -21383,7 +21383,7 @@
     </row>
     <row r="545" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A545">
-        <v>441202000</v>
+        <v>43021226000</v>
       </c>
       <c r="B545">
         <v>18487</v>
@@ -21409,7 +21409,7 @@
     </row>
     <row r="546" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A546">
-        <v>441202000</v>
+        <v>43021226000</v>
       </c>
       <c r="B546">
         <v>18602</v>

</xml_diff>

<commit_message>
Reorganized into ischemic heart disease (include stable and unstable)
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -6057,7 +6057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E544" sqref="E544"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13443,7 +13443,7 @@
     </row>
     <row r="262" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262">
-        <v>312327000</v>
+        <v>4185932000</v>
       </c>
       <c r="B262">
         <v>17379</v>
@@ -13472,7 +13472,7 @@
     </row>
     <row r="263" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>312327000</v>
+        <v>4185932000</v>
       </c>
       <c r="B263">
         <v>17378</v>
@@ -13501,7 +13501,7 @@
     </row>
     <row r="264" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264">
-        <v>312327000</v>
+        <v>4185932000</v>
       </c>
       <c r="B264">
         <v>17753</v>
@@ -13527,7 +13527,7 @@
     </row>
     <row r="265" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265">
-        <v>312327000</v>
+        <v>4185932000</v>
       </c>
       <c r="B265">
         <v>18935</v>
@@ -15223,7 +15223,7 @@
       </c>
     </row>
     <row r="326" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="2">
+      <c r="A326">
         <v>4185932000</v>
       </c>
       <c r="B326">
@@ -15252,7 +15252,7 @@
       </c>
     </row>
     <row r="327" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A327" s="2">
+      <c r="A327">
         <v>4185932000</v>
       </c>
       <c r="B327">
@@ -15281,7 +15281,7 @@
       </c>
     </row>
     <row r="328" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A328" s="2">
+      <c r="A328">
         <v>4185932000</v>
       </c>
       <c r="B328">
@@ -15307,7 +15307,7 @@
       </c>
     </row>
     <row r="329" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A329" s="2">
+      <c r="A329">
         <v>4185932000</v>
       </c>
       <c r="B329">

</xml_diff>

<commit_message>
Move asthma into hypersensitivity disorder
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -6057,7 +6057,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="D302" sqref="D302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14487,8 +14487,8 @@
       </c>
     </row>
     <row r="300" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A300">
-        <v>317009000</v>
+      <c r="A300" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B300">
         <v>17411</v>
@@ -14516,8 +14516,8 @@
       </c>
     </row>
     <row r="301" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A301">
-        <v>317009000</v>
+      <c r="A301" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B301">
         <v>17410</v>
@@ -14545,8 +14545,8 @@
       </c>
     </row>
     <row r="302" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A302">
-        <v>317009000</v>
+      <c r="A302" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B302">
         <v>17741</v>
@@ -14571,8 +14571,8 @@
       </c>
     </row>
     <row r="303" spans="1:10" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A303">
-        <v>317009000</v>
+      <c r="A303" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B303">
         <v>17767</v>
@@ -14597,8 +14597,8 @@
       </c>
     </row>
     <row r="304" spans="1:10" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A304">
-        <v>317009000</v>
+      <c r="A304" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B304">
         <v>17768</v>
@@ -14623,8 +14623,8 @@
       </c>
     </row>
     <row r="305" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A305">
-        <v>317009000</v>
+      <c r="A305" s="2">
+        <v>43021226000</v>
       </c>
       <c r="B305">
         <v>18775</v>

</xml_diff>

<commit_message>
Anemia, thrombocytopenia, leukopenia to cellular components
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -5243,7 +5243,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5383,6 +5383,12 @@
       <color rgb="FF24292E"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -5726,12 +5732,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6057,7 +6064,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D302" sqref="D302"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17494,8 +17501,8 @@
       </c>
     </row>
     <row r="407" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A407">
-        <v>432870000</v>
+      <c r="A407" s="3">
+        <v>443723000</v>
       </c>
       <c r="B407">
         <v>17689</v>
@@ -17523,8 +17530,8 @@
       </c>
     </row>
     <row r="408" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A408">
-        <v>432870000</v>
+      <c r="A408" s="3">
+        <v>443723000</v>
       </c>
       <c r="B408">
         <v>17688</v>
@@ -17552,8 +17559,8 @@
       </c>
     </row>
     <row r="409" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A409">
-        <v>432870000</v>
+      <c r="A409" s="3">
+        <v>443723000</v>
       </c>
       <c r="B409">
         <v>18573</v>
@@ -17578,8 +17585,8 @@
       </c>
     </row>
     <row r="410" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A410">
-        <v>432870000</v>
+      <c r="A410" s="3">
+        <v>443723000</v>
       </c>
       <c r="B410">
         <v>18576</v>
@@ -17604,8 +17611,8 @@
       </c>
     </row>
     <row r="411" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A411">
-        <v>432881000</v>
+      <c r="A411" s="3">
+        <v>443723000</v>
       </c>
       <c r="B411">
         <v>17617</v>
@@ -17633,8 +17640,8 @@
       </c>
     </row>
     <row r="412" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A412">
-        <v>432881000</v>
+      <c r="A412" s="3">
+        <v>443723000</v>
       </c>
       <c r="B412">
         <v>17616</v>
@@ -18308,8 +18315,8 @@
       </c>
     </row>
     <row r="436" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A436">
-        <v>435224000</v>
+      <c r="A436" s="3">
+        <v>443723000</v>
       </c>
       <c r="B436">
         <v>17547</v>
@@ -18337,8 +18344,8 @@
       </c>
     </row>
     <row r="437" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A437">
-        <v>435224000</v>
+      <c r="A437" s="3">
+        <v>443723000</v>
       </c>
       <c r="B437">
         <v>17546</v>
@@ -20621,7 +20628,7 @@
     </row>
     <row r="518" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A518">
-        <v>439777000</v>
+        <v>443723000</v>
       </c>
       <c r="B518">
         <v>17399</v>
@@ -20650,7 +20657,7 @@
     </row>
     <row r="519" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A519">
-        <v>439777000</v>
+        <v>443723000</v>
       </c>
       <c r="B519">
         <v>17398</v>

</xml_diff>

<commit_message>
Deprecated myocarditis and pericarditis and added to Inflammatory of disorder of mediastinum
</commit_message>
<xml_diff>
--- a/extras/CohortDescription.xlsx
+++ b/extras/CohortDescription.xlsx
@@ -8474,7 +8474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D666" sqref="D666"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17598,7 +17598,7 @@
     </row>
     <row r="288" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288">
-        <v>314383000</v>
+        <v>4189294000</v>
       </c>
       <c r="B288">
         <v>18675</v>
@@ -17630,7 +17630,7 @@
     </row>
     <row r="289" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289">
-        <v>314383000</v>
+        <v>4189294000</v>
       </c>
       <c r="B289">
         <v>18674</v>
@@ -17662,7 +17662,7 @@
     </row>
     <row r="290" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290">
-        <v>314383000</v>
+        <v>4189294000</v>
       </c>
       <c r="B290">
         <v>18520</v>
@@ -17691,7 +17691,7 @@
     </row>
     <row r="291" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291">
-        <v>314383000</v>
+        <v>4189294000</v>
       </c>
       <c r="B291">
         <v>18579</v>
@@ -29390,7 +29390,7 @@
     </row>
     <row r="664" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A664">
-        <v>4138837000</v>
+        <v>4189294000</v>
       </c>
       <c r="B664">
         <v>17623</v>
@@ -29422,7 +29422,7 @@
     </row>
     <row r="665" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A665">
-        <v>4138837000</v>
+        <v>4189294000</v>
       </c>
       <c r="B665">
         <v>17622</v>
@@ -29454,7 +29454,7 @@
     </row>
     <row r="666" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A666">
-        <v>4138837000</v>
+        <v>4189294000</v>
       </c>
       <c r="B666">
         <v>18522</v>
@@ -29483,7 +29483,7 @@
     </row>
     <row r="667" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A667">
-        <v>4138837000</v>
+        <v>4189294000</v>
       </c>
       <c r="B667">
         <v>18557</v>

</xml_diff>